<commit_message>
added a template page with the form and other stuff... and now you can either send a json or fill the form from this personal web page.
</commit_message>
<xml_diff>
--- a/UserInfo.xlsx
+++ b/UserInfo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,24 +448,30 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ewrwr fgfsfsdfs</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3234234</v>
-      </c>
-      <c r="C5" t="n">
-        <v>54</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3234234</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Standard Bank</t>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>qeqweqw dasda</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>3123</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>132123</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2312</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>eqwweq</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added therequirements.txt file to help.
</commit_message>
<xml_diff>
--- a/UserInfo.xlsx
+++ b/UserInfo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,30 +448,30 @@
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>qeqweqw dasda</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>3123</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>132123</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2312</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>eqwweq</t>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sdadad 2313</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>23132</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1231</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2312321</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>stand</t>
         </is>
       </c>
     </row>

</xml_diff>